<commit_message>
updaite livrable 1 table utilisateur
</commit_message>
<xml_diff>
--- a/livrable 1/POO_dictionnaire_de_données.xlsx
+++ b/livrable 1/POO_dictionnaire_de_données.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viacesifr-my.sharepoint.com/personal/willy_carlot_viacesi_fr/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBAF1182-A2AB-4420-8F6B-D79FD95DFCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11B0EBE7-7B91-493A-8B6B-A60F0CD83A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{D6F570DF-6BBB-4554-82C7-64FA371B2255}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="85">
   <si>
     <t xml:space="preserve">variable </t>
   </si>
@@ -254,25 +254,28 @@
     <t>code postal de l'adresse</t>
   </si>
   <si>
-    <t>humain</t>
+    <t>utilisateur</t>
+  </si>
+  <si>
+    <t>id_utilisateur</t>
   </si>
   <si>
     <t>id de l'humain</t>
   </si>
   <si>
-    <t>hum_nom</t>
+    <t>uti_nom</t>
   </si>
   <si>
     <t>nom de l'humain</t>
   </si>
   <si>
-    <t>hum_prenom</t>
+    <t>uti_prenom</t>
   </si>
   <si>
     <t>prenom de l'humain</t>
   </si>
   <si>
-    <t>hum_dateNaissance</t>
+    <t>uti_dateNaissance</t>
   </si>
   <si>
     <t>date de naissance de l'humain</t>
@@ -745,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57CA384-A9C6-4618-ABF3-E72534924F85}">
   <dimension ref="B3:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F34"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="68" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -1579,7 +1582,7 @@
         <v>72</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>13</v>
@@ -1588,13 +1591,13 @@
         <v>4</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H29" t="s">
         <v>72</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>16</v>
@@ -1616,7 +1619,7 @@
     </row>
     <row r="30" spans="2:18" ht="15">
       <c r="C30" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>25</v>
@@ -1625,10 +1628,10 @@
         <v>50</v>
       </c>
       <c r="F30" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -1644,7 +1647,7 @@
     </row>
     <row r="31" spans="2:18" ht="15">
       <c r="C31" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>25</v>
@@ -1653,10 +1656,10 @@
         <v>50</v>
       </c>
       <c r="F31" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
@@ -1672,7 +1675,7 @@
     </row>
     <row r="32" spans="2:18">
       <c r="C32" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>18</v>
@@ -1681,10 +1684,10 @@
         <v>8</v>
       </c>
       <c r="F32" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
@@ -1700,7 +1703,7 @@
     </row>
     <row r="33" spans="2:18" ht="15">
       <c r="B33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>12</v>
@@ -1712,10 +1715,10 @@
         <v>4</v>
       </c>
       <c r="F33" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" t="s">
         <v>81</v>
-      </c>
-      <c r="H33" t="s">
-        <v>80</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>12</v>
@@ -1736,7 +1739,7 @@
     </row>
     <row r="34" spans="2:18">
       <c r="C34" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>25</v>
@@ -1745,10 +1748,10 @@
         <v>50</v>
       </c>
       <c r="F34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I34" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>82</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
@@ -1803,14 +1806,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c7e9659a-247f-4fc5-b96b-8066ebefd750" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CED5A00CDE64C14FB88C5AB9CF307A73" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c6e841309374518167bbe31246b7f48b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c7e9659a-247f-4fc5-b96b-8066ebefd750" xmlns:ns4="408cb695-034b-4c51-96e3-b8f77eb66ab8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="be754f26bf5494740491075ac44b9f36" ns3:_="" ns4:_="">
     <xsd:import namespace="c7e9659a-247f-4fc5-b96b-8066ebefd750"/>
@@ -1999,7 +1994,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2008,14 +2003,22 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c7e9659a-247f-4fc5-b96b-8066ebefd750" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B670C240-BD7A-4AF1-8AEC-2BC72CFCA3C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F292855-2BB8-4F1D-BC38-64C0CEA000E5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F292855-2BB8-4F1D-BC38-64C0CEA000E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0208C915-D208-4401-83A7-625E350C8B52}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0208C915-D208-4401-83A7-625E350C8B52}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B670C240-BD7A-4AF1-8AEC-2BC72CFCA3C7}"/>
 </file>
</xml_diff>